<commit_message>
nvda earnigns and tech update
</commit_message>
<xml_diff>
--- a/NVDA/NVDA Model - (02-14-2024).xlsx
+++ b/NVDA/NVDA Model - (02-14-2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buzz5\OneDrive\Desktop\FModels\NVDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94370C99-B955-49AE-9EDD-E20ECA0BDBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89573CFD-EC75-4091-BA51-D7F440132EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86DED09B-2833-4D69-AD50-3DC99F242132}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{86DED09B-2833-4D69-AD50-3DC99F242132}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="117">
   <si>
     <t>ALL IN $ USD</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>TSMC makes NVIDIA chips</t>
+  </si>
+  <si>
+    <t>FY24</t>
   </si>
 </sst>
 </file>
@@ -776,43 +779,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A915255-7085-4C22-945C-1F53AB87465D}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f ca="1">TODAY()</f>
-        <v>45336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -822,22 +824,22 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -848,7 +850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -856,7 +858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
@@ -864,7 +866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
@@ -872,185 +874,201 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4">
         <v>26000</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="4"/>
+      <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>26</v>
       </c>
       <c r="E17">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="4">
-        <v>2468</v>
-      </c>
-      <c r="G18" s="3" t="s">
+        <v>2490</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="4">
         <f>E18*E17</f>
-        <v>1779428</v>
-      </c>
-      <c r="H19" t="s">
+        <v>1964610</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="I19" t="s">
         <v>101</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="4">
-        <v>13296</v>
-      </c>
-      <c r="H20" t="s">
+        <f>25984</f>
+        <v>25984</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" t="s">
         <v>102</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="4">
-        <v>10605</v>
-      </c>
-      <c r="H21" t="s">
+        <f>8549+1119+2541</f>
+        <v>12209</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" t="s">
         <v>103</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="4">
         <f>E19-E20+E21</f>
-        <v>1776737</v>
-      </c>
-      <c r="H22" t="s">
+        <v>1950835</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="I22" t="s">
         <v>104</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="4">
         <v>22160</v>
       </c>
-      <c r="H23" t="s">
+      <c r="F23" s="4"/>
+      <c r="I23" t="s">
         <v>105</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="4">
         <f>E22/E23</f>
-        <v>80.177662454873641</v>
-      </c>
-      <c r="H24" t="s">
+        <v>88.034070397111918</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="I24" t="s">
         <v>106</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1067,11 +1085,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B207C8-9AB3-4D32-81A5-CB52CE47C6B0}">
   <dimension ref="A1:FH26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AA5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI13" sqref="AI13"/>
+      <selection pane="bottomRight" activeCell="AS16" sqref="AS16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,6 +1336,30 @@
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
+      <c r="BT4">
+        <f t="shared" ref="BT4" si="1">BS4+1</f>
+        <v>2045</v>
+      </c>
+      <c r="BU4">
+        <f t="shared" ref="BU4" si="2">BT4+1</f>
+        <v>2046</v>
+      </c>
+      <c r="BV4">
+        <f t="shared" ref="BV4" si="3">BU4+1</f>
+        <v>2047</v>
+      </c>
+      <c r="BW4">
+        <f t="shared" ref="BW4" si="4">BV4+1</f>
+        <v>2048</v>
+      </c>
+      <c r="BX4">
+        <f t="shared" ref="BX4" si="5">BW4+1</f>
+        <v>2049</v>
+      </c>
+      <c r="BY4">
+        <f t="shared" ref="BY4" si="6">BX4+1</f>
+        <v>2050</v>
+      </c>
     </row>
     <row r="5" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
@@ -1410,7 +1452,9 @@
       <c r="AE5" s="4">
         <v>18120</v>
       </c>
-      <c r="AF5" s="4"/>
+      <c r="AF5" s="4">
+        <v>22103</v>
+      </c>
       <c r="AG5" s="4"/>
       <c r="AH5" s="9" t="s">
         <v>84</v>
@@ -1461,6 +1505,10 @@
         <f>SUM(Y5:AB5)</f>
         <v>26974</v>
       </c>
+      <c r="AY5" s="4">
+        <f>SUM(AC5:AF5)</f>
+        <v>60922</v>
+      </c>
     </row>
     <row r="6" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
@@ -1553,13 +1601,15 @@
       <c r="AE6" s="4">
         <v>4720</v>
       </c>
-      <c r="AF6" s="4"/>
+      <c r="AF6" s="4">
+        <v>5312</v>
+      </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4" t="s">
         <v>92</v>
       </c>
       <c r="AI6" s="10">
-        <v>0.08</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
@@ -1606,6 +1656,10 @@
         <f>SUM(Y6:AB6)</f>
         <v>11618</v>
       </c>
+      <c r="AY6" s="4">
+        <f t="shared" ref="AY6:AY12" si="7">SUM(AC6:AF6)</f>
+        <v>16621</v>
+      </c>
     </row>
     <row r="7" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
@@ -1616,119 +1670,119 @@
         <v>1150</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:X7" si="1">F5-F6</f>
+        <f t="shared" ref="F7:X7" si="8">F5-F6</f>
         <v>1302</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1569</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1801</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>2068</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1975</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1921</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1207</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1296</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1541</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>1916</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>2015</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>2004</v>
       </c>
       <c r="R7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>2275</v>
       </c>
       <c r="S7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>2510</v>
       </c>
       <c r="T7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>3607</v>
       </c>
       <c r="U7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>3629</v>
       </c>
       <c r="V7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4215</v>
       </c>
       <c r="W7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4631</v>
       </c>
       <c r="X7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>5000</v>
       </c>
       <c r="Y7" s="4">
-        <f t="shared" ref="Y7" si="2">Y5-Y6</f>
+        <f t="shared" ref="Y7" si="9">Y5-Y6</f>
         <v>5431</v>
       </c>
       <c r="Z7" s="4">
-        <f t="shared" ref="Z7" si="3">Z5-Z6</f>
+        <f t="shared" ref="Z7" si="10">Z5-Z6</f>
         <v>2915</v>
       </c>
       <c r="AA7" s="4">
-        <f t="shared" ref="AA7" si="4">AA5-AA6</f>
+        <f t="shared" ref="AA7" si="11">AA5-AA6</f>
         <v>3177</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" ref="AB7" si="5">AB5-AB6</f>
+        <f t="shared" ref="AB7" si="12">AB5-AB6</f>
         <v>3833</v>
       </c>
       <c r="AC7" s="4">
-        <f t="shared" ref="AC7" si="6">AC5-AC6</f>
+        <f t="shared" ref="AC7" si="13">AC5-AC6</f>
         <v>4648</v>
       </c>
       <c r="AD7" s="4">
-        <f t="shared" ref="AD7" si="7">AD5-AD6</f>
+        <f t="shared" ref="AD7" si="14">AD5-AD6</f>
         <v>9462</v>
       </c>
       <c r="AE7" s="4">
-        <f t="shared" ref="AE7" si="8">AE5-AE6</f>
+        <f t="shared" ref="AE7" si="15">AE5-AE6</f>
         <v>13400</v>
       </c>
       <c r="AF7" s="4">
-        <f t="shared" ref="AF7" si="9">AF5-AF6</f>
-        <v>0</v>
+        <f t="shared" ref="AF7" si="16">AF5-AF6</f>
+        <v>16791</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4" t="s">
         <v>91</v>
       </c>
       <c r="AI7" s="10">
-        <v>6.5000000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="AJ7" s="4"/>
       <c r="AK7" s="4"/>
@@ -1737,54 +1791,57 @@
         <v>1409</v>
       </c>
       <c r="AM7" s="4">
-        <f t="shared" ref="AM7:AX7" si="10">AM5-AM6</f>
+        <f t="shared" ref="AM7:AX7" si="17">AM5-AM6</f>
         <v>2059</v>
       </c>
       <c r="AN7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2227</v>
       </c>
       <c r="AO7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2268</v>
       </c>
       <c r="AP7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2599</v>
       </c>
       <c r="AQ7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>7171</v>
       </c>
       <c r="AR7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>6768</v>
       </c>
       <c r="AS7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>5822</v>
       </c>
       <c r="AT7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>7171</v>
       </c>
       <c r="AU7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>6768</v>
       </c>
       <c r="AV7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>16082</v>
       </c>
       <c r="AW7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>17475</v>
       </c>
       <c r="AX7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>15356</v>
       </c>
-      <c r="AY7" s="4"/>
+      <c r="AY7" s="4">
+        <f t="shared" si="7"/>
+        <v>44301</v>
+      </c>
       <c r="AZ7" s="4"/>
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
@@ -1883,14 +1940,16 @@
       <c r="AE8" s="4">
         <v>2983</v>
       </c>
-      <c r="AF8" s="4"/>
+      <c r="AF8" s="4">
+        <v>3176</v>
+      </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="9" t="s">
         <v>85</v>
       </c>
       <c r="AI8" s="4">
         <f>NPV(AI7,AL13:FH13)</f>
-        <v>567665.79106775171</v>
+        <v>2126884.6904602223</v>
       </c>
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
@@ -1937,6 +1996,10 @@
         <f>SUM(Y8:AB8)</f>
         <v>11132</v>
       </c>
+      <c r="AY8" s="4">
+        <f t="shared" si="7"/>
+        <v>11329</v>
+      </c>
     </row>
     <row r="9" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
@@ -1947,112 +2010,112 @@
         <v>554</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" ref="F9:X9" si="11">F7-F8</f>
+        <f t="shared" ref="F9:X9" si="18">F7-F8</f>
         <v>688</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>895</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1073</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1295</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1157</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1058</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>294</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>358</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>571</v>
       </c>
       <c r="O9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>927</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>990</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>976</v>
       </c>
       <c r="R9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>651</v>
       </c>
       <c r="S9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>948</v>
       </c>
       <c r="T9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1957</v>
       </c>
       <c r="U9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1956</v>
       </c>
       <c r="V9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>2444</v>
       </c>
       <c r="W9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>2671</v>
       </c>
       <c r="X9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>2970</v>
       </c>
       <c r="Y9" s="4">
-        <f t="shared" ref="Y9" si="12">Y7-Y8</f>
+        <f t="shared" ref="Y9" si="19">Y7-Y8</f>
         <v>3563</v>
       </c>
       <c r="Z9" s="4">
-        <f t="shared" ref="Z9" si="13">Z7-Z8</f>
+        <f t="shared" ref="Z9" si="20">Z7-Z8</f>
         <v>499</v>
       </c>
       <c r="AA9" s="4">
-        <f t="shared" ref="AA9" si="14">AA7-AA8</f>
+        <f t="shared" ref="AA9" si="21">AA7-AA8</f>
         <v>601</v>
       </c>
       <c r="AB9" s="4">
-        <f t="shared" ref="AB9" si="15">AB7-AB8</f>
+        <f t="shared" ref="AB9" si="22">AB7-AB8</f>
         <v>-439</v>
       </c>
       <c r="AC9" s="4">
-        <f t="shared" ref="AC9" si="16">AC7-AC8</f>
+        <f t="shared" ref="AC9" si="23">AC7-AC8</f>
         <v>2140</v>
       </c>
       <c r="AD9" s="4">
-        <f t="shared" ref="AD9" si="17">AD7-AD8</f>
+        <f t="shared" ref="AD9" si="24">AD7-AD8</f>
         <v>6800</v>
       </c>
       <c r="AE9" s="4">
-        <f t="shared" ref="AE9" si="18">AE7-AE8</f>
+        <f t="shared" ref="AE9" si="25">AE7-AE8</f>
         <v>10417</v>
       </c>
       <c r="AF9" s="4">
-        <f t="shared" ref="AF9" si="19">AF7-AF8</f>
-        <v>0</v>
+        <f t="shared" ref="AF9" si="26">AF7-AF8</f>
+        <v>13615</v>
       </c>
       <c r="AG9" s="4"/>
       <c r="AH9" s="4" t="s">
@@ -2060,63 +2123,66 @@
       </c>
       <c r="AI9" s="4">
         <f>Main!E20-Model!E21</f>
-        <v>13296</v>
+        <v>25984</v>
       </c>
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4">
-        <f t="shared" ref="AL9:AX9" si="20">AL7-AL8</f>
+        <f t="shared" ref="AL9:AX9" si="27">AL7-AL8</f>
         <v>256</v>
       </c>
       <c r="AM9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>651</v>
       </c>
       <c r="AN9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>649</v>
       </c>
       <c r="AO9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>497</v>
       </c>
       <c r="AP9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>759</v>
       </c>
       <c r="AQ9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>3804</v>
       </c>
       <c r="AR9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>2846</v>
       </c>
       <c r="AS9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>3210</v>
       </c>
       <c r="AT9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>3804</v>
       </c>
       <c r="AU9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>2846</v>
       </c>
       <c r="AV9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>9028</v>
       </c>
       <c r="AW9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>10041</v>
       </c>
       <c r="AX9" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>4224</v>
       </c>
-      <c r="AY9" s="4"/>
+      <c r="AY9" s="4">
+        <f t="shared" si="7"/>
+        <v>32972</v>
+      </c>
       <c r="AZ9" s="4"/>
       <c r="BA9" s="4"/>
       <c r="BB9" s="4"/>
@@ -2215,14 +2281,17 @@
       <c r="AE10" s="4">
         <v>105</v>
       </c>
-      <c r="AF10" s="4"/>
+      <c r="AF10" s="4">
+        <f>294-63+260</f>
+        <v>491</v>
+      </c>
       <c r="AG10" s="4"/>
       <c r="AH10" s="9" t="s">
         <v>87</v>
       </c>
       <c r="AI10" s="4">
         <f>AI8+AI9</f>
-        <v>580961.79106775171</v>
+        <v>2152868.6904602223</v>
       </c>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
@@ -2275,6 +2344,10 @@
         <f>SUM(Y10:AB10)</f>
         <v>-43</v>
       </c>
+      <c r="AY10" s="4">
+        <f t="shared" si="7"/>
+        <v>846</v>
+      </c>
     </row>
     <row r="11" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
@@ -2285,112 +2358,112 @@
         <v>536</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:X11" si="21">F9+F10</f>
+        <f t="shared" ref="F11:X11" si="28">F9+F10</f>
         <v>684</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>894</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1050</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1311</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1180</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1081</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>324</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>389</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>606</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>959</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1016</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>981</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>609</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>898</v>
       </c>
       <c r="T11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>1921</v>
       </c>
       <c r="U11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>2044</v>
       </c>
       <c r="V11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>2394</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>2638</v>
       </c>
       <c r="X11" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>2865</v>
       </c>
       <c r="Y11" s="4">
-        <f t="shared" ref="Y11" si="22">Y9+Y10</f>
+        <f t="shared" ref="Y11" si="29">Y9+Y10</f>
         <v>3500</v>
       </c>
       <c r="Z11" s="4">
-        <f t="shared" ref="Z11" si="23">Z9+Z10</f>
+        <f t="shared" ref="Z11" si="30">Z9+Z10</f>
         <v>475</v>
       </c>
       <c r="AA11" s="4">
-        <f t="shared" ref="AA11" si="24">AA9+AA10</f>
+        <f t="shared" ref="AA11" si="31">AA9+AA10</f>
         <v>613</v>
       </c>
       <c r="AB11" s="4">
-        <f t="shared" ref="AB11" si="25">AB9+AB10</f>
+        <f t="shared" ref="AB11" si="32">AB9+AB10</f>
         <v>-407</v>
       </c>
       <c r="AC11" s="4">
-        <f t="shared" ref="AC11" si="26">AC9+AC10</f>
+        <f t="shared" ref="AC11" si="33">AC9+AC10</f>
         <v>2209</v>
       </c>
       <c r="AD11" s="4">
-        <f t="shared" ref="AD11" si="27">AD9+AD10</f>
+        <f t="shared" ref="AD11" si="34">AD9+AD10</f>
         <v>6981</v>
       </c>
       <c r="AE11" s="4">
-        <f t="shared" ref="AE11" si="28">AE9+AE10</f>
+        <f t="shared" ref="AE11" si="35">AE9+AE10</f>
         <v>10522</v>
       </c>
       <c r="AF11" s="4">
-        <f t="shared" ref="AF11" si="29">AF9+AF10</f>
-        <v>0</v>
+        <f t="shared" ref="AF11" si="36">AF9+AF10</f>
+        <v>14106</v>
       </c>
       <c r="AG11" s="4"/>
       <c r="AH11" s="4"/>
@@ -2398,58 +2471,61 @@
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4">
-        <f t="shared" ref="AL11:AX11" si="30">AL9+AL10</f>
+        <f t="shared" ref="AL11:AX11" si="37">AL9+AL10</f>
         <v>271</v>
       </c>
       <c r="AM11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>667</v>
       </c>
       <c r="AN11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>663</v>
       </c>
       <c r="AO11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>512</v>
       </c>
       <c r="AP11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>769</v>
       </c>
       <c r="AQ11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>3896</v>
       </c>
       <c r="AR11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>2970</v>
       </c>
       <c r="AS11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>3196</v>
       </c>
       <c r="AT11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>3896</v>
       </c>
       <c r="AU11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>2970</v>
       </c>
       <c r="AV11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>8997</v>
       </c>
       <c r="AW11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>9941</v>
       </c>
       <c r="AX11" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>4181</v>
       </c>
-      <c r="AY11" s="4"/>
+      <c r="AY11" s="4">
+        <f t="shared" si="7"/>
+        <v>33818</v>
+      </c>
       <c r="AZ11" s="4"/>
       <c r="BA11" s="4"/>
       <c r="BB11" s="4"/>
@@ -2548,14 +2624,16 @@
       <c r="AE12" s="4">
         <v>1279</v>
       </c>
-      <c r="AF12" s="4"/>
+      <c r="AF12" s="4">
+        <v>1821</v>
+      </c>
       <c r="AG12" s="4"/>
       <c r="AH12" s="9" t="s">
         <v>90</v>
       </c>
       <c r="AI12" s="4">
         <f>Main!E17</f>
-        <v>721</v>
+        <v>789</v>
       </c>
       <c r="AJ12" s="4"/>
       <c r="AK12" s="4"/>
@@ -2602,6 +2680,10 @@
         <f>SUM(Y12:AB12)</f>
         <v>-187</v>
       </c>
+      <c r="AY12" s="4">
+        <f t="shared" si="7"/>
+        <v>4059</v>
+      </c>
     </row>
     <row r="13" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
@@ -2612,112 +2694,112 @@
         <v>507</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" ref="F13:X13" si="31">F11-F12</f>
+        <f t="shared" ref="F13:X13" si="38">F11-F12</f>
         <v>583</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>836</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1089</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1244</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1101</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1230</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>569</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>394</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>552</v>
       </c>
       <c r="O13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>899</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>961</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>917</v>
       </c>
       <c r="R13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>622</v>
       </c>
       <c r="S13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>886</v>
       </c>
       <c r="T13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1933</v>
       </c>
       <c r="U13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>1912</v>
       </c>
       <c r="V13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2374</v>
       </c>
       <c r="W13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2464</v>
       </c>
       <c r="X13" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>3002</v>
       </c>
       <c r="Y13" s="4">
-        <f t="shared" ref="Y13" si="32">Y11-Y12</f>
+        <f t="shared" ref="Y13" si="39">Y11-Y12</f>
         <v>3313</v>
       </c>
       <c r="Z13" s="4">
-        <f t="shared" ref="Z13" si="33">Z11-Z12</f>
+        <f t="shared" ref="Z13" si="40">Z11-Z12</f>
         <v>656</v>
       </c>
       <c r="AA13" s="4">
-        <f t="shared" ref="AA13" si="34">AA11-AA12</f>
+        <f t="shared" ref="AA13" si="41">AA11-AA12</f>
         <v>680</v>
       </c>
       <c r="AB13" s="4">
-        <f t="shared" ref="AB13" si="35">AB11-AB12</f>
+        <f t="shared" ref="AB13" si="42">AB11-AB12</f>
         <v>-281</v>
       </c>
       <c r="AC13" s="4">
-        <f t="shared" ref="AC13" si="36">AC11-AC12</f>
+        <f t="shared" ref="AC13" si="43">AC11-AC12</f>
         <v>2043</v>
       </c>
       <c r="AD13" s="4">
-        <f t="shared" ref="AD13" si="37">AD11-AD12</f>
+        <f t="shared" ref="AD13" si="44">AD11-AD12</f>
         <v>6188</v>
       </c>
       <c r="AE13" s="4">
-        <f t="shared" ref="AE13" si="38">AE11-AE12</f>
+        <f t="shared" ref="AE13" si="45">AE11-AE12</f>
         <v>9243</v>
       </c>
       <c r="AF13" s="4">
-        <f t="shared" ref="AF13" si="39">AF11-AF12</f>
-        <v>0</v>
+        <f t="shared" ref="AF13" si="46">AF11-AF12</f>
+        <v>12285</v>
       </c>
       <c r="AG13" s="4"/>
       <c r="AH13" s="9" t="s">
@@ -2725,518 +2807,377 @@
       </c>
       <c r="AI13" s="4">
         <f>AI10/Main!E18</f>
-        <v>235.39780837429163</v>
+        <v>864.60589978322184</v>
       </c>
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4">
-        <f t="shared" ref="AL13:AX13" si="40">AL11-AL12</f>
+        <f t="shared" ref="AL13:AY15" si="47">AL11-AL12</f>
         <v>253</v>
       </c>
       <c r="AM13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>585</v>
       </c>
       <c r="AN13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>564</v>
       </c>
       <c r="AO13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>442</v>
       </c>
       <c r="AP13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>639</v>
       </c>
       <c r="AQ13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>4141</v>
       </c>
       <c r="AR13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>2796</v>
       </c>
       <c r="AS13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>3047</v>
       </c>
       <c r="AT13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>4141</v>
       </c>
       <c r="AU13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>2806</v>
       </c>
       <c r="AV13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>8683</v>
       </c>
       <c r="AW13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>9752</v>
       </c>
       <c r="AX13" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>4368</v>
       </c>
       <c r="AY13" s="4">
-        <f>AX13*($AI$6+1)</f>
-        <v>4717.4400000000005</v>
+        <f t="shared" si="47"/>
+        <v>29759</v>
       </c>
       <c r="AZ13" s="4">
-        <f t="shared" ref="AZ13:DK13" si="41">AY13*($AI$6+1)</f>
-        <v>5094.8352000000004</v>
+        <f t="shared" ref="AZ13:DK13" si="48">AY13*($AI$6+1)</f>
+        <v>32288.514999999999</v>
       </c>
       <c r="BA13" s="4">
-        <f t="shared" si="41"/>
-        <v>5502.4220160000004</v>
+        <f t="shared" si="48"/>
+        <v>35033.038775000001</v>
       </c>
       <c r="BB13" s="4">
-        <f t="shared" si="41"/>
-        <v>5942.6157772800007</v>
+        <f t="shared" si="48"/>
+        <v>38010.847070875003</v>
       </c>
       <c r="BC13" s="4">
-        <f t="shared" si="41"/>
-        <v>6418.0250394624009</v>
+        <f t="shared" si="48"/>
+        <v>41241.769071899376</v>
       </c>
       <c r="BD13" s="4">
-        <f t="shared" si="41"/>
-        <v>6931.4670426193934</v>
+        <f t="shared" si="48"/>
+        <v>44747.31944301082</v>
       </c>
       <c r="BE13" s="4">
-        <f t="shared" si="41"/>
-        <v>7485.9844060289452</v>
+        <f t="shared" si="48"/>
+        <v>48550.841595666738</v>
       </c>
       <c r="BF13" s="4">
-        <f t="shared" si="41"/>
-        <v>8084.8631585112616</v>
+        <f t="shared" si="48"/>
+        <v>52677.66313129841</v>
       </c>
       <c r="BG13" s="4">
-        <f t="shared" si="41"/>
-        <v>8731.652211192164</v>
+        <f t="shared" si="48"/>
+        <v>57155.264497458775</v>
       </c>
       <c r="BH13" s="4">
-        <f t="shared" si="41"/>
-        <v>9430.1843880875385</v>
+        <f t="shared" si="48"/>
+        <v>62013.461979742766</v>
       </c>
       <c r="BI13" s="4">
-        <f t="shared" si="41"/>
-        <v>10184.599139134541</v>
+        <f t="shared" si="48"/>
+        <v>67284.606248020893</v>
       </c>
       <c r="BJ13" s="4">
-        <f t="shared" si="41"/>
-        <v>10999.367070265305</v>
+        <f t="shared" si="48"/>
+        <v>73003.797779102664</v>
       </c>
       <c r="BK13" s="4">
-        <f t="shared" si="41"/>
-        <v>11879.316435886531</v>
+        <f t="shared" si="48"/>
+        <v>79209.120590326391</v>
       </c>
       <c r="BL13" s="4">
-        <f t="shared" si="41"/>
-        <v>12829.661750757454</v>
+        <f t="shared" si="48"/>
+        <v>85941.895840504134</v>
       </c>
       <c r="BM13" s="4">
-        <f t="shared" si="41"/>
-        <v>13856.034690818051</v>
+        <f t="shared" si="48"/>
+        <v>93246.956986946985</v>
       </c>
       <c r="BN13" s="4">
-        <f t="shared" si="41"/>
-        <v>14964.517466083496</v>
+        <f t="shared" si="48"/>
+        <v>101172.94833083748</v>
       </c>
       <c r="BO13" s="4">
-        <f t="shared" si="41"/>
-        <v>16161.678863370178</v>
+        <f t="shared" si="48"/>
+        <v>109772.64893895866</v>
       </c>
       <c r="BP13" s="4">
-        <f t="shared" si="41"/>
-        <v>17454.613172439793</v>
+        <f t="shared" si="48"/>
+        <v>119103.32409877014</v>
       </c>
       <c r="BQ13" s="4">
-        <f t="shared" si="41"/>
-        <v>18850.982226234977</v>
+        <f t="shared" si="48"/>
+        <v>129227.10664716559</v>
       </c>
       <c r="BR13" s="4">
-        <f t="shared" si="41"/>
-        <v>20359.060804333778</v>
+        <f t="shared" si="48"/>
+        <v>140211.41071217466</v>
       </c>
       <c r="BS13" s="4">
-        <f t="shared" si="41"/>
-        <v>21987.785668680481</v>
+        <f t="shared" si="48"/>
+        <v>152129.38062270952</v>
       </c>
       <c r="BT13" s="4">
-        <f t="shared" si="41"/>
-        <v>23746.808522174921</v>
+        <f t="shared" si="48"/>
+        <v>165060.37797563983</v>
       </c>
       <c r="BU13" s="4">
-        <f t="shared" si="41"/>
-        <v>25646.553203948915</v>
+        <f t="shared" si="48"/>
+        <v>179090.51010356922</v>
       </c>
       <c r="BV13" s="4">
-        <f t="shared" si="41"/>
-        <v>27698.277460264831</v>
+        <f t="shared" si="48"/>
+        <v>194313.20346237259</v>
       </c>
       <c r="BW13" s="4">
-        <f t="shared" si="41"/>
-        <v>29914.13965708602</v>
+        <f t="shared" si="48"/>
+        <v>210829.82575667425</v>
       </c>
       <c r="BX13" s="4">
-        <f t="shared" si="41"/>
-        <v>32307.270829652902</v>
+        <f t="shared" si="48"/>
+        <v>228750.36094599156</v>
       </c>
       <c r="BY13" s="4">
-        <f t="shared" si="41"/>
-        <v>34891.852496025138</v>
+        <f t="shared" si="48"/>
+        <v>248194.14162640084</v>
       </c>
       <c r="BZ13" s="4">
-        <f t="shared" si="41"/>
-        <v>37683.20069570715</v>
+        <f t="shared" ref="BZ13" si="49">BY13*($AI$6+1)</f>
+        <v>269290.64366464491</v>
       </c>
       <c r="CA13" s="4">
-        <f t="shared" si="41"/>
-        <v>40697.856751363724</v>
+        <f t="shared" ref="CA13" si="50">BZ13*($AI$6+1)</f>
+        <v>292180.34837613971</v>
       </c>
       <c r="CB13" s="4">
-        <f t="shared" si="41"/>
-        <v>43953.685291472822</v>
+        <f t="shared" ref="CB13" si="51">CA13*($AI$6+1)</f>
+        <v>317015.67798811157</v>
       </c>
       <c r="CC13" s="4">
-        <f t="shared" si="41"/>
-        <v>47469.980114790655</v>
+        <f t="shared" ref="CC13" si="52">CB13*($AI$6+1)</f>
+        <v>343962.01061710104</v>
       </c>
       <c r="CD13" s="4">
-        <f t="shared" si="41"/>
-        <v>51267.578523973913</v>
+        <f t="shared" ref="CD13" si="53">CC13*($AI$6+1)</f>
+        <v>373198.78151955461</v>
       </c>
       <c r="CE13" s="4">
-        <f t="shared" si="41"/>
-        <v>55368.984805891829</v>
+        <f t="shared" ref="CE13" si="54">CD13*($AI$6+1)</f>
+        <v>404920.67794871674</v>
       </c>
       <c r="CF13" s="4">
-        <f t="shared" si="41"/>
-        <v>59798.50359036318</v>
+        <f t="shared" ref="CF13" si="55">CE13*($AI$6+1)</f>
+        <v>439338.93557435763</v>
       </c>
       <c r="CG13" s="4">
-        <f t="shared" si="41"/>
-        <v>64582.383877592241</v>
+        <f t="shared" ref="CG13" si="56">CF13*($AI$6+1)</f>
+        <v>476682.74509817804</v>
       </c>
       <c r="CH13" s="4">
-        <f t="shared" si="41"/>
-        <v>69748.974587799632</v>
+        <f t="shared" ref="CH13" si="57">CG13*($AI$6+1)</f>
+        <v>517200.77843152318</v>
       </c>
       <c r="CI13" s="4">
-        <f t="shared" si="41"/>
-        <v>75328.892554823615</v>
+        <f t="shared" ref="CI13" si="58">CH13*($AI$6+1)</f>
+        <v>561162.84459820262</v>
       </c>
       <c r="CJ13" s="4">
-        <f t="shared" si="41"/>
-        <v>81355.20395920951</v>
+        <f t="shared" ref="CJ13" si="59">CI13*($AI$6+1)</f>
+        <v>608861.68638904986</v>
       </c>
       <c r="CK13" s="4">
-        <f t="shared" si="41"/>
-        <v>87863.620275946276</v>
+        <f t="shared" ref="CK13" si="60">CJ13*($AI$6+1)</f>
+        <v>660614.92973211908</v>
       </c>
       <c r="CL13" s="4">
-        <f t="shared" si="41"/>
-        <v>94892.709898021989</v>
+        <f t="shared" ref="CL13" si="61">CK13*($AI$6+1)</f>
+        <v>716767.19875934918</v>
       </c>
       <c r="CM13" s="4">
-        <f t="shared" si="41"/>
-        <v>102484.12668986376</v>
+        <f t="shared" ref="CM13" si="62">CL13*($AI$6+1)</f>
+        <v>777692.41065389384</v>
       </c>
       <c r="CN13" s="4">
-        <f t="shared" si="41"/>
-        <v>110682.85682505286</v>
+        <f t="shared" ref="CN13" si="63">CM13*($AI$6+1)</f>
+        <v>843796.26555947482</v>
       </c>
       <c r="CO13" s="4">
-        <f t="shared" si="41"/>
-        <v>119537.4853710571</v>
+        <f t="shared" ref="CO13" si="64">CN13*($AI$6+1)</f>
+        <v>915518.9481320302</v>
       </c>
       <c r="CP13" s="4">
-        <f t="shared" si="41"/>
-        <v>129100.48420074169</v>
+        <f t="shared" ref="CP13" si="65">CO13*($AI$6+1)</f>
+        <v>993338.05872325273</v>
       </c>
       <c r="CQ13" s="4">
-        <f t="shared" si="41"/>
-        <v>139428.52293680102</v>
+        <f t="shared" ref="CQ13" si="66">CP13*($AI$6+1)</f>
+        <v>1077771.7937147291</v>
       </c>
       <c r="CR13" s="4">
-        <f t="shared" si="41"/>
-        <v>150582.80477174511</v>
+        <f t="shared" ref="CR13" si="67">CQ13*($AI$6+1)</f>
+        <v>1169382.3961804812</v>
       </c>
       <c r="CS13" s="4">
-        <f t="shared" si="41"/>
-        <v>162629.42915348473</v>
+        <f t="shared" ref="CS13" si="68">CR13*($AI$6+1)</f>
+        <v>1268779.8998558221</v>
       </c>
       <c r="CT13" s="4">
-        <f t="shared" si="41"/>
-        <v>175639.78348576353</v>
+        <f t="shared" ref="CT13" si="69">CS13*($AI$6+1)</f>
+        <v>1376626.1913435669</v>
       </c>
       <c r="CU13" s="4">
-        <f t="shared" si="41"/>
-        <v>189690.96616462464</v>
+        <f t="shared" ref="CU13" si="70">CT13*($AI$6+1)</f>
+        <v>1493639.4176077701</v>
       </c>
       <c r="CV13" s="4">
-        <f t="shared" si="41"/>
-        <v>204866.24345779463</v>
+        <f t="shared" ref="CV13" si="71">CU13*($AI$6+1)</f>
+        <v>1620598.7681044305</v>
       </c>
       <c r="CW13" s="4">
-        <f t="shared" si="41"/>
-        <v>221255.54293441822</v>
+        <f t="shared" ref="CW13" si="72">CV13*($AI$6+1)</f>
+        <v>1758349.663393307</v>
       </c>
       <c r="CX13" s="4">
-        <f t="shared" si="41"/>
-        <v>238955.9863691717</v>
+        <f t="shared" ref="CX13" si="73">CW13*($AI$6+1)</f>
+        <v>1907809.384781738</v>
       </c>
       <c r="CY13" s="4">
-        <f t="shared" si="41"/>
-        <v>258072.46527870547</v>
+        <f t="shared" ref="CY13" si="74">CX13*($AI$6+1)</f>
+        <v>2069973.1824881858</v>
       </c>
       <c r="CZ13" s="4">
-        <f t="shared" si="41"/>
-        <v>278718.26250100194</v>
+        <f t="shared" ref="CZ13" si="75">CY13*($AI$6+1)</f>
+        <v>2245920.9029996814</v>
       </c>
       <c r="DA13" s="4">
-        <f t="shared" si="41"/>
-        <v>301015.7235010821</v>
+        <f t="shared" ref="DA13" si="76">CZ13*($AI$6+1)</f>
+        <v>2436824.1797546544</v>
       </c>
       <c r="DB13" s="4">
-        <f t="shared" si="41"/>
-        <v>325096.98138116871</v>
+        <f t="shared" ref="DB13" si="77">DA13*($AI$6+1)</f>
+        <v>2643954.2350337999</v>
       </c>
       <c r="DC13" s="4">
-        <f t="shared" si="41"/>
-        <v>351104.7398916622</v>
+        <f t="shared" ref="DC13" si="78">DB13*($AI$6+1)</f>
+        <v>2868690.3450116729</v>
       </c>
       <c r="DD13" s="4">
-        <f t="shared" si="41"/>
-        <v>379193.11908299522</v>
+        <f t="shared" ref="DD13" si="79">DC13*($AI$6+1)</f>
+        <v>3112529.0243376652</v>
       </c>
       <c r="DE13" s="4">
-        <f t="shared" si="41"/>
-        <v>409528.56860963488</v>
+        <f t="shared" ref="DE13" si="80">DD13*($AI$6+1)</f>
+        <v>3377093.9914063667</v>
       </c>
       <c r="DF13" s="4">
-        <f t="shared" si="41"/>
-        <v>442290.85409840569</v>
+        <f t="shared" ref="DF13" si="81">DE13*($AI$6+1)</f>
+        <v>3664146.9806759078</v>
       </c>
       <c r="DG13" s="4">
-        <f t="shared" si="41"/>
-        <v>477674.12242627819</v>
+        <f t="shared" ref="DG13" si="82">DF13*($AI$6+1)</f>
+        <v>3975599.4740333599</v>
       </c>
       <c r="DH13" s="4">
-        <f t="shared" si="41"/>
-        <v>515888.05222038046</v>
+        <f t="shared" ref="DH13" si="83">DG13*($AI$6+1)</f>
+        <v>4313525.4293261953</v>
       </c>
       <c r="DI13" s="4">
-        <f t="shared" si="41"/>
-        <v>557159.09639801097</v>
+        <f t="shared" ref="DI13" si="84">DH13*($AI$6+1)</f>
+        <v>4680175.090818922</v>
       </c>
       <c r="DJ13" s="4">
-        <f t="shared" si="41"/>
-        <v>601731.82410985185</v>
+        <f t="shared" ref="DJ13" si="85">DI13*($AI$6+1)</f>
+        <v>5077989.9735385301</v>
       </c>
       <c r="DK13" s="4">
-        <f t="shared" si="41"/>
-        <v>649870.37003863999</v>
+        <f t="shared" ref="DK13" si="86">DJ13*($AI$6+1)</f>
+        <v>5509619.1212893054</v>
       </c>
       <c r="DL13" s="4">
-        <f t="shared" ref="DL13:FH13" si="42">DK13*($AI$6+1)</f>
-        <v>701859.99964173127</v>
+        <f t="shared" ref="DL13" si="87">DK13*($AI$6+1)</f>
+        <v>5977936.7465988966</v>
       </c>
       <c r="DM13" s="4">
-        <f t="shared" si="42"/>
-        <v>758008.79961306986</v>
-      </c>
-      <c r="DN13" s="4">
-        <f t="shared" si="42"/>
-        <v>818649.50358211552</v>
-      </c>
-      <c r="DO13" s="4">
-        <f t="shared" si="42"/>
-        <v>884141.46386868483</v>
-      </c>
-      <c r="DP13" s="4">
-        <f t="shared" si="42"/>
-        <v>954872.78097817965</v>
-      </c>
-      <c r="DQ13" s="4">
-        <f t="shared" si="42"/>
-        <v>1031262.6034564341</v>
-      </c>
-      <c r="DR13" s="4">
-        <f t="shared" si="42"/>
-        <v>1113763.6117329488</v>
-      </c>
-      <c r="DS13" s="4">
-        <f t="shared" si="42"/>
-        <v>1202864.7006715848</v>
-      </c>
-      <c r="DT13" s="4">
-        <f t="shared" si="42"/>
-        <v>1299093.8767253116</v>
-      </c>
-      <c r="DU13" s="4">
-        <f t="shared" si="42"/>
-        <v>1403021.3868633367</v>
-      </c>
-      <c r="DV13" s="4">
-        <f t="shared" si="42"/>
-        <v>1515263.0978124037</v>
-      </c>
-      <c r="DW13" s="4">
-        <f t="shared" si="42"/>
-        <v>1636484.145637396</v>
-      </c>
-      <c r="DX13" s="4">
-        <f t="shared" si="42"/>
-        <v>1767402.8772883879</v>
-      </c>
-      <c r="DY13" s="4">
-        <f t="shared" si="42"/>
-        <v>1908795.1074714591</v>
-      </c>
-      <c r="DZ13" s="4">
-        <f t="shared" si="42"/>
-        <v>2061498.7160691759</v>
-      </c>
-      <c r="EA13" s="4">
-        <f t="shared" si="42"/>
-        <v>2226418.6133547099</v>
-      </c>
-      <c r="EB13" s="4">
-        <f t="shared" si="42"/>
-        <v>2404532.1024230868</v>
-      </c>
-      <c r="EC13" s="4">
-        <f t="shared" si="42"/>
-        <v>2596894.6706169341</v>
-      </c>
-      <c r="ED13" s="4">
-        <f t="shared" si="42"/>
-        <v>2804646.2442662888</v>
-      </c>
-      <c r="EE13" s="4">
-        <f t="shared" si="42"/>
-        <v>3029017.9438075921</v>
-      </c>
-      <c r="EF13" s="4">
-        <f t="shared" si="42"/>
-        <v>3271339.3793121995</v>
-      </c>
-      <c r="EG13" s="4">
-        <f t="shared" si="42"/>
-        <v>3533046.5296571758</v>
-      </c>
-      <c r="EH13" s="4">
-        <f t="shared" si="42"/>
-        <v>3815690.25202975</v>
-      </c>
-      <c r="EI13" s="4">
-        <f t="shared" si="42"/>
-        <v>4120945.4721921305</v>
-      </c>
-      <c r="EJ13" s="4">
-        <f t="shared" si="42"/>
-        <v>4450621.1099675009</v>
-      </c>
-      <c r="EK13" s="4">
-        <f t="shared" si="42"/>
-        <v>4806670.7987649012</v>
-      </c>
-      <c r="EL13" s="4">
-        <f t="shared" si="42"/>
-        <v>5191204.4626660934</v>
-      </c>
-      <c r="EM13" s="4">
-        <f t="shared" si="42"/>
-        <v>5606500.8196793813</v>
-      </c>
-      <c r="EN13" s="4">
-        <f t="shared" si="42"/>
-        <v>6055020.8852537321</v>
-      </c>
-      <c r="EO13" s="4">
-        <f t="shared" si="42"/>
-        <v>6539422.5560740307</v>
-      </c>
-      <c r="EP13" s="4">
-        <f t="shared" si="42"/>
-        <v>7062576.3605599534</v>
-      </c>
-      <c r="EQ13" s="4">
-        <f t="shared" si="42"/>
-        <v>7627582.4694047505</v>
-      </c>
-      <c r="ER13" s="4">
-        <f t="shared" si="42"/>
-        <v>8237789.066957131</v>
-      </c>
-      <c r="ES13" s="4">
-        <f t="shared" si="42"/>
-        <v>8896812.1923137028</v>
-      </c>
-      <c r="ET13" s="4">
-        <f t="shared" si="42"/>
-        <v>9608557.1676987987</v>
-      </c>
-      <c r="EU13" s="4">
-        <f t="shared" si="42"/>
-        <v>10377241.741114704</v>
-      </c>
-      <c r="EV13" s="4">
-        <f t="shared" si="42"/>
-        <v>11207421.080403881</v>
-      </c>
-      <c r="EW13" s="4">
-        <f t="shared" si="42"/>
-        <v>12104014.766836192</v>
-      </c>
-      <c r="EX13" s="4">
-        <f t="shared" si="42"/>
-        <v>13072335.948183089</v>
-      </c>
-      <c r="EY13" s="4">
-        <f t="shared" si="42"/>
-        <v>14118122.824037738</v>
-      </c>
-      <c r="EZ13" s="4">
-        <f t="shared" si="42"/>
-        <v>15247572.649960758</v>
-      </c>
-      <c r="FA13" s="4">
-        <f t="shared" si="42"/>
-        <v>16467378.46195762</v>
-      </c>
-      <c r="FB13" s="4">
-        <f t="shared" si="42"/>
-        <v>17784768.738914233</v>
-      </c>
-      <c r="FC13" s="4">
-        <f t="shared" si="42"/>
-        <v>19207550.238027371</v>
-      </c>
-      <c r="FD13" s="4">
-        <f t="shared" si="42"/>
-        <v>20744154.257069562</v>
-      </c>
-      <c r="FE13" s="4">
-        <f t="shared" si="42"/>
-        <v>22403686.597635128</v>
-      </c>
-      <c r="FF13" s="4">
-        <f t="shared" si="42"/>
-        <v>24195981.525445938</v>
-      </c>
-      <c r="FG13" s="4">
-        <f t="shared" si="42"/>
-        <v>26131660.047481615</v>
-      </c>
-      <c r="FH13" s="4">
-        <f t="shared" si="42"/>
-        <v>28222192.851280145</v>
-      </c>
+        <f t="shared" ref="DM13" si="88">DL13*($AI$6+1)</f>
+        <v>6486061.3700598022</v>
+      </c>
+      <c r="DN13" s="4"/>
+      <c r="DO13" s="4"/>
+      <c r="DP13" s="4"/>
+      <c r="DQ13" s="4"/>
+      <c r="DR13" s="4"/>
+      <c r="DS13" s="4"/>
+      <c r="DT13" s="4"/>
+      <c r="DU13" s="4"/>
+      <c r="DV13" s="4"/>
+      <c r="DW13" s="4"/>
+      <c r="DX13" s="4"/>
+      <c r="DY13" s="4"/>
+      <c r="DZ13" s="4"/>
+      <c r="EA13" s="4"/>
+      <c r="EB13" s="4"/>
+      <c r="EC13" s="4"/>
+      <c r="ED13" s="4"/>
+      <c r="EE13" s="4"/>
+      <c r="EF13" s="4"/>
+      <c r="EG13" s="4"/>
+      <c r="EH13" s="4"/>
+      <c r="EI13" s="4"/>
+      <c r="EJ13" s="4"/>
+      <c r="EK13" s="4"/>
+      <c r="EL13" s="4"/>
+      <c r="EM13" s="4"/>
+      <c r="EN13" s="4"/>
+      <c r="EO13" s="4"/>
+      <c r="EP13" s="4"/>
+      <c r="EQ13" s="4"/>
+      <c r="ER13" s="4"/>
+      <c r="ES13" s="4"/>
+      <c r="ET13" s="4"/>
+      <c r="EU13" s="4"/>
+      <c r="EV13" s="4"/>
+      <c r="EW13" s="4"/>
+      <c r="EX13" s="4"/>
+      <c r="EY13" s="4"/>
+      <c r="EZ13" s="4"/>
+      <c r="FA13" s="4"/>
+      <c r="FB13" s="4"/>
+      <c r="FC13" s="4"/>
+      <c r="FD13" s="4"/>
+      <c r="FE13" s="4"/>
+      <c r="FF13" s="4"/>
+      <c r="FG13" s="4"/>
+      <c r="FH13" s="4"/>
     </row>
     <row r="14" spans="1:164" x14ac:dyDescent="0.25">
       <c r="D14" s="3"/>
@@ -3274,7 +3215,7 @@
       </c>
       <c r="AI14" s="10">
         <f>AI13/AI12-1</f>
-        <v>-0.67351205495937361</v>
+        <v>9.5824968039571301E-2</v>
       </c>
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
@@ -3382,26 +3323,49 @@
       <c r="AE15" s="6">
         <v>3.75</v>
       </c>
-      <c r="AF15" s="6"/>
+      <c r="AF15" s="6">
+        <v>4.93</v>
+      </c>
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="6"/>
-      <c r="AL15" s="6"/>
+      <c r="AL15" s="4"/>
       <c r="AM15" s="6"/>
       <c r="AN15" s="6"/>
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="6"/>
       <c r="AR15" s="6"/>
-      <c r="AS15" s="6"/>
-      <c r="AT15" s="6"/>
-      <c r="AU15" s="6"/>
-      <c r="AV15" s="6"/>
-      <c r="AW15" s="6"/>
-      <c r="AX15" s="6"/>
-      <c r="AY15" s="6"/>
+      <c r="AS15" s="4">
+        <f t="shared" ref="AS15:AT15" si="89">SUM(K15:N15)</f>
+        <v>4.62</v>
+      </c>
+      <c r="AT15" s="4">
+        <f t="shared" si="89"/>
+        <v>4.07</v>
+      </c>
+      <c r="AU15" s="4">
+        <f>SUM(M15:P15)</f>
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="AV15" s="4">
+        <f t="shared" ref="AV15:AY15" si="90">SUM(N15:Q15)</f>
+        <v>5.35</v>
+      </c>
+      <c r="AW15" s="4">
+        <f t="shared" si="90"/>
+        <v>5.43</v>
+      </c>
+      <c r="AX15" s="4">
+        <f t="shared" si="90"/>
+        <v>6.08</v>
+      </c>
+      <c r="AY15" s="4">
+        <f t="shared" si="90"/>
+        <v>6.9</v>
+      </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
@@ -3500,7 +3464,9 @@
       <c r="AE16" s="4">
         <v>2494</v>
       </c>
-      <c r="AF16" s="4"/>
+      <c r="AF16" s="4">
+        <v>2490</v>
+      </c>
       <c r="AG16" s="4"/>
       <c r="AH16" s="4"/>
       <c r="AI16" s="4"/>
@@ -3566,91 +3532,91 @@
         <v>0.14990138067061154</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" ref="G19:AE19" si="43">G13/F13-1</f>
+        <f t="shared" ref="G19:AF19" si="91">G13/F13-1</f>
         <v>0.4339622641509433</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.30263157894736836</v>
       </c>
       <c r="I19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.14233241505968786</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-0.114951768488746</v>
       </c>
       <c r="K19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.11716621253406001</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-0.5373983739837398</v>
       </c>
       <c r="M19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-0.30755711775043937</v>
       </c>
       <c r="N19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.40101522842639592</v>
       </c>
       <c r="O19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.62862318840579712</v>
       </c>
       <c r="P19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>6.8965517241379226E-2</v>
       </c>
       <c r="Q19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-4.57856399583767E-2</v>
       </c>
       <c r="R19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-0.32170119956379495</v>
       </c>
       <c r="S19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.42443729903536975</v>
       </c>
       <c r="T19" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>1.1817155756207676</v>
       </c>
       <c r="U19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-1.0863942058975673E-2</v>
       </c>
       <c r="V19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.24163179916318001</v>
       </c>
       <c r="W19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>3.7910699241785917E-2</v>
       </c>
       <c r="X19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.2183441558441559</v>
       </c>
       <c r="Y19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.10359760159893394</v>
       </c>
       <c r="Z19" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-0.8019921521279807</v>
       </c>
       <c r="AA19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>3.6585365853658569E-2</v>
       </c>
       <c r="AB19" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>-1.4132352941176469</v>
       </c>
       <c r="AC19" s="7">
@@ -3658,14 +3624,17 @@
         <v>-8.270462633451956</v>
       </c>
       <c r="AD19" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>2.0288790993636807</v>
       </c>
       <c r="AE19" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="91"/>
         <v>0.49369747899159666</v>
       </c>
-      <c r="AF19" s="8"/>
+      <c r="AF19" s="8">
+        <f t="shared" si="91"/>
+        <v>0.32911392405063289</v>
+      </c>
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
       <c r="AI19" s="8"/>
@@ -3673,54 +3642,57 @@
       <c r="AK19" s="8"/>
       <c r="AL19" s="8"/>
       <c r="AM19" s="8">
-        <f t="shared" ref="AM19" si="44">AM13/AL13-1</f>
+        <f t="shared" ref="AM19" si="92">AM13/AL13-1</f>
         <v>1.3122529644268774</v>
       </c>
       <c r="AN19" s="8">
-        <f t="shared" ref="AN19" si="45">AN13/AM13-1</f>
+        <f t="shared" ref="AN19" si="93">AN13/AM13-1</f>
         <v>-3.5897435897435881E-2</v>
       </c>
       <c r="AO19" s="8">
-        <f t="shared" ref="AO19" si="46">AO13/AN13-1</f>
+        <f t="shared" ref="AO19" si="94">AO13/AN13-1</f>
         <v>-0.21631205673758869</v>
       </c>
       <c r="AP19" s="8">
-        <f t="shared" ref="AP19" si="47">AP13/AO13-1</f>
+        <f t="shared" ref="AP19" si="95">AP13/AO13-1</f>
         <v>0.44570135746606332</v>
       </c>
       <c r="AQ19" s="8">
-        <f t="shared" ref="AQ19" si="48">AQ13/AP13-1</f>
+        <f t="shared" ref="AQ19" si="96">AQ13/AP13-1</f>
         <v>5.4804381846635364</v>
       </c>
       <c r="AR19" s="8">
-        <f t="shared" ref="AR19" si="49">AR13/AQ13-1</f>
+        <f t="shared" ref="AR19" si="97">AR13/AQ13-1</f>
         <v>-0.3248007727602028</v>
       </c>
       <c r="AS19" s="8">
-        <f t="shared" ref="AS19" si="50">AS13/AR13-1</f>
+        <f t="shared" ref="AS19" si="98">AS13/AR13-1</f>
         <v>8.9771101573676626E-2</v>
       </c>
       <c r="AT19" s="8">
-        <f t="shared" ref="AT19" si="51">AT13/AS13-1</f>
+        <f t="shared" ref="AT19" si="99">AT13/AS13-1</f>
         <v>0.35904168034131922</v>
       </c>
       <c r="AU19" s="8">
-        <f t="shared" ref="AU19" si="52">AU13/AT13-1</f>
+        <f t="shared" ref="AU19" si="100">AU13/AT13-1</f>
         <v>-0.32238589712629795</v>
       </c>
       <c r="AV19" s="8">
-        <f t="shared" ref="AV19" si="53">AV13/AU13-1</f>
+        <f t="shared" ref="AV19" si="101">AV13/AU13-1</f>
         <v>2.0944404846756948</v>
       </c>
       <c r="AW19" s="8">
-        <f t="shared" ref="AW19" si="54">AW13/AV13-1</f>
+        <f t="shared" ref="AW19" si="102">AW13/AV13-1</f>
         <v>0.12311413106069335</v>
       </c>
       <c r="AX19" s="8">
-        <f t="shared" ref="AX19" si="55">AX13/AW13-1</f>
+        <f t="shared" ref="AX19:AY19" si="103">AX13/AW13-1</f>
         <v>-0.55209187858900743</v>
       </c>
-      <c r="AY19" s="8"/>
+      <c r="AY19" s="8">
+        <f t="shared" si="103"/>
+        <v>5.8129578754578759</v>
+      </c>
       <c r="AZ19" s="8"/>
       <c r="BA19" s="8"/>
       <c r="BB19" s="8"/>
@@ -3743,106 +3715,109 @@
         <v>0.15126484254001027</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" ref="G20:AE20" si="56">G5/F5-1</f>
+        <f t="shared" ref="G20:AF20" si="104">G5/F5-1</f>
         <v>0.1820627802690582</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.10432473444613044</v>
       </c>
       <c r="I20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.1016832703538304</v>
       </c>
       <c r="J20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>-2.6192703461178635E-2</v>
       </c>
       <c r="K20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>1.8571886007044514E-2</v>
       </c>
       <c r="L20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>-0.30682175416535684</v>
       </c>
       <c r="M20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>6.8027210884353817E-3</v>
       </c>
       <c r="N20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.16171171171171173</v>
       </c>
       <c r="O20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.16867002714230317</v>
       </c>
       <c r="P20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>3.0192435301924281E-2</v>
       </c>
       <c r="Q20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>-8.0515297906602612E-3</v>
       </c>
       <c r="R20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.2551948051948052</v>
       </c>
       <c r="S20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.10605276771857208</v>
       </c>
       <c r="T20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.27525724976613652</v>
       </c>
       <c r="U20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>3.8144140839904583E-2</v>
       </c>
       <c r="V20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.14944356120826718</v>
       </c>
       <c r="W20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>9.1593668357153879E-2</v>
       </c>
       <c r="X20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>7.6024215120371608E-2</v>
       </c>
       <c r="Y20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>8.4390945963626951E-2</v>
       </c>
       <c r="Z20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>-0.19111969111969107</v>
       </c>
       <c r="AA20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>-0.11530429594272074</v>
       </c>
       <c r="AB20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>2.0232675771370667E-2</v>
       </c>
       <c r="AC20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.1885638737398776</v>
       </c>
       <c r="AD20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.87805895439377091</v>
       </c>
       <c r="AE20" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="104"/>
         <v>0.34152661582882948</v>
       </c>
-      <c r="AF20" s="8"/>
+      <c r="AF20" s="8">
+        <f t="shared" si="104"/>
+        <v>0.21981236203090515</v>
+      </c>
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
       <c r="AI20" s="8"/>
@@ -3850,54 +3825,57 @@
       <c r="AK20" s="8"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8">
-        <f t="shared" ref="AM20" si="57">AM5/AL5-1</f>
+        <f t="shared" ref="AM20" si="105">AM5/AL5-1</f>
         <v>0.12898673440587083</v>
       </c>
       <c r="AN20" s="8">
-        <f t="shared" ref="AN20" si="58">AN5/AM5-1</f>
+        <f t="shared" ref="AN20" si="106">AN5/AM5-1</f>
         <v>7.0000000000000062E-2</v>
       </c>
       <c r="AO20" s="8">
-        <f t="shared" ref="AO20" si="59">AO5/AN5-1</f>
+        <f t="shared" ref="AO20" si="107">AO5/AN5-1</f>
         <v>-3.5046728971962593E-2</v>
       </c>
       <c r="AP20" s="8">
-        <f t="shared" ref="AP20" si="60">AP5/AO5-1</f>
+        <f t="shared" ref="AP20" si="108">AP5/AO5-1</f>
         <v>0.13341404358353515</v>
       </c>
       <c r="AQ20" s="8">
-        <f t="shared" ref="AQ20" si="61">AQ5/AP5-1</f>
+        <f t="shared" ref="AQ20" si="109">AQ5/AP5-1</f>
         <v>1.5028839991454817</v>
       </c>
       <c r="AR20" s="8">
-        <f t="shared" ref="AR20" si="62">AR5/AQ5-1</f>
+        <f t="shared" ref="AR20" si="110">AR5/AQ5-1</f>
         <v>-6.8111983612154314E-2</v>
       </c>
       <c r="AS20" s="8">
-        <f t="shared" ref="AS20" si="63">AS5/AR5-1</f>
+        <f t="shared" ref="AS20" si="111">AS5/AR5-1</f>
         <v>-0.11027660743725953</v>
       </c>
       <c r="AT20" s="8">
-        <f t="shared" ref="AT20" si="64">AT5/AS5-1</f>
+        <f t="shared" ref="AT20" si="112">AT5/AS5-1</f>
         <v>0.20609429689108505</v>
       </c>
       <c r="AU20" s="8">
-        <f t="shared" ref="AU20" si="65">AU5/AT5-1</f>
+        <f t="shared" ref="AU20" si="113">AU5/AT5-1</f>
         <v>-6.8111983612154314E-2</v>
       </c>
       <c r="AV20" s="8">
-        <f t="shared" ref="AV20" si="66">AV5/AU5-1</f>
+        <f t="shared" ref="AV20" si="114">AV5/AU5-1</f>
         <v>1.2645173108627952</v>
       </c>
       <c r="AW20" s="8">
-        <f t="shared" ref="AW20" si="67">AW5/AV5-1</f>
+        <f t="shared" ref="AW20" si="115">AW5/AV5-1</f>
         <v>8.8577900016178601E-2</v>
       </c>
       <c r="AX20" s="8">
-        <f t="shared" ref="AX20" si="68">AX5/AW5-1</f>
+        <f t="shared" ref="AX20:AY20" si="116">AX5/AW5-1</f>
         <v>2.2293230289069932E-3</v>
       </c>
-      <c r="AY20" s="8"/>
+      <c r="AY20" s="8">
+        <f t="shared" si="116"/>
+        <v>1.2585452658115224</v>
+      </c>
       <c r="AZ20" s="8"/>
       <c r="BA20" s="8"/>
       <c r="BB20" s="8"/>
@@ -3920,106 +3898,109 @@
         <v>3.0201342281879207E-2</v>
       </c>
       <c r="G21" s="8">
-        <f t="shared" ref="G21:AE21" si="69">G8/F8-1</f>
+        <f t="shared" ref="G21:AF21" si="117">G8/F8-1</f>
         <v>9.7719869706840434E-2</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>8.0118694362017795E-2</v>
       </c>
       <c r="I21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>6.1813186813186816E-2</v>
       </c>
       <c r="J21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>5.8214747736093253E-2</v>
       </c>
       <c r="K21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>5.5012224938875365E-2</v>
       </c>
       <c r="L21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>5.7937427578215628E-2</v>
       </c>
       <c r="M21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>2.7382256297918905E-2</v>
       </c>
       <c r="N21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>3.4115138592750505E-2</v>
       </c>
       <c r="O21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>1.9587628865979312E-2</v>
       </c>
       <c r="P21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>3.6400404448938328E-2</v>
       </c>
       <c r="Q21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>2.9268292682926855E-3</v>
       </c>
       <c r="R21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>0.57976653696498048</v>
       </c>
       <c r="S21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>-3.8177339901477869E-2</v>
       </c>
       <c r="T21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>5.6338028169014009E-2</v>
       </c>
       <c r="U21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>1.3939393939393918E-2</v>
       </c>
       <c r="V21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>5.8577405857740628E-2</v>
       </c>
       <c r="W21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>0.10671936758893286</v>
       </c>
       <c r="X21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>3.5714285714285809E-2</v>
       </c>
       <c r="Y21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>-7.98029556650246E-2</v>
       </c>
       <c r="Z21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>0.29336188436830835</v>
       </c>
       <c r="AA21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>6.6225165562913801E-2</v>
       </c>
       <c r="AB21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>0.65838509316770177</v>
       </c>
       <c r="AC21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>-0.4129213483146067</v>
       </c>
       <c r="AD21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>6.1403508771929793E-2</v>
       </c>
       <c r="AE21" s="8">
-        <f t="shared" si="69"/>
+        <f t="shared" si="117"/>
         <v>0.12058602554470332</v>
       </c>
-      <c r="AF21" s="8"/>
+      <c r="AF21" s="8">
+        <f t="shared" si="117"/>
+        <v>6.4699966476701398E-2</v>
+      </c>
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
@@ -4027,54 +4008,57 @@
       <c r="AK21" s="8"/>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8">
-        <f t="shared" ref="AM21" si="70">AM8/AL8-1</f>
+        <f t="shared" ref="AM21" si="118">AM8/AL8-1</f>
         <v>0.22116218560277545</v>
       </c>
       <c r="AN21" s="8">
-        <f t="shared" ref="AN21" si="71">AN8/AM8-1</f>
+        <f t="shared" ref="AN21" si="119">AN8/AM8-1</f>
         <v>0.12073863636363646</v>
       </c>
       <c r="AO21" s="8">
-        <f t="shared" ref="AO21" si="72">AO8/AN8-1</f>
+        <f t="shared" ref="AO21" si="120">AO8/AN8-1</f>
         <v>0.12230671736375154</v>
       </c>
       <c r="AP21" s="8">
-        <f t="shared" ref="AP21" si="73">AP8/AO8-1</f>
+        <f t="shared" ref="AP21" si="121">AP8/AO8-1</f>
         <v>3.8961038961038863E-2</v>
       </c>
       <c r="AQ21" s="8">
-        <f t="shared" ref="AQ21" si="74">AQ8/AP8-1</f>
+        <f t="shared" ref="AQ21" si="122">AQ8/AP8-1</f>
         <v>0.82989130434782599</v>
       </c>
       <c r="AR21" s="8">
-        <f t="shared" ref="AR21" si="75">AR8/AQ8-1</f>
+        <f t="shared" ref="AR21" si="123">AR8/AQ8-1</f>
         <v>0.16483516483516492</v>
       </c>
       <c r="AS21" s="8">
-        <f t="shared" ref="AS21" si="76">AS8/AR8-1</f>
+        <f t="shared" ref="AS21" si="124">AS8/AR8-1</f>
         <v>-0.33401325854156039</v>
       </c>
       <c r="AT21" s="8">
-        <f t="shared" ref="AT21" si="77">AT8/AS8-1</f>
+        <f t="shared" ref="AT21" si="125">AT8/AS8-1</f>
         <v>0.28905053598774888</v>
       </c>
       <c r="AU21" s="8">
-        <f t="shared" ref="AU21" si="78">AU8/AT8-1</f>
+        <f t="shared" ref="AU21" si="126">AU8/AT8-1</f>
         <v>0.16483516483516492</v>
       </c>
       <c r="AV21" s="8">
-        <f t="shared" ref="AV21" si="79">AV8/AU8-1</f>
+        <f t="shared" ref="AV21" si="127">AV8/AU8-1</f>
         <v>0.79857215706272311</v>
       </c>
       <c r="AW21" s="8">
-        <f t="shared" ref="AW21" si="80">AW8/AV8-1</f>
+        <f t="shared" ref="AW21" si="128">AW8/AV8-1</f>
         <v>5.3870144598809233E-2</v>
       </c>
       <c r="AX21" s="8">
-        <f t="shared" ref="AX21" si="81">AX8/AW8-1</f>
+        <f t="shared" ref="AX21:AY21" si="129">AX8/AW8-1</f>
         <v>0.49744417541027719</v>
       </c>
-      <c r="AY21" s="8"/>
+      <c r="AY21" s="8">
+        <f t="shared" si="129"/>
+        <v>1.7696730147322981E-2</v>
+      </c>
       <c r="AZ21" s="8"/>
       <c r="BA21" s="8"/>
       <c r="BB21" s="8"/>
@@ -4100,164 +4084,170 @@
         <v>0.58385650224215246</v>
       </c>
       <c r="G22" s="8">
-        <f t="shared" ref="G22:AE22" si="82">G7/G5</f>
+        <f t="shared" ref="G22:AE22" si="130">G7/G5</f>
         <v>0.59522003034901361</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.61868773617313633</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.6448394137823511</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.63240473903298111</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.60389814523734675</v>
       </c>
       <c r="L22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.54739229024943314</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.58378378378378382</v>
       </c>
       <c r="N22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.59751841799146954</v>
       </c>
       <c r="O22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.63570006635700071</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.64895330112721417</v>
       </c>
       <c r="Q22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.6506493506493507</v>
       </c>
       <c r="R22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.58846352819451631</v>
       </c>
       <c r="S22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.58699719363891489</v>
       </c>
       <c r="T22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.66147075004584632</v>
       </c>
       <c r="U22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.6410528175234057</v>
       </c>
       <c r="V22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.64776394651913327</v>
       </c>
       <c r="W22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.65197803744896521</v>
       </c>
       <c r="X22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.65419337956299883</v>
       </c>
       <c r="Y22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.65528474903474898</v>
       </c>
       <c r="Z22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.43481503579952269</v>
       </c>
       <c r="AA22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.53566009104704093</v>
       </c>
       <c r="AB22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.63344901669145592</v>
       </c>
       <c r="AC22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.64627363737486099</v>
       </c>
       <c r="AD22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.7005256533649219</v>
       </c>
       <c r="AE22" s="8">
-        <f t="shared" si="82"/>
+        <f t="shared" si="130"/>
         <v>0.73951434878587197</v>
       </c>
-      <c r="AF22" s="8"/>
+      <c r="AF22" s="8">
+        <f t="shared" ref="AF22" si="131">AF7/AF5</f>
+        <v>0.75967063294575399</v>
+      </c>
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
       <c r="AK22" s="8"/>
       <c r="AL22" s="8">
-        <f t="shared" ref="AL22:AX22" si="83">AL7/AL5</f>
+        <f t="shared" ref="AL22:AX22" si="132">AL7/AL5</f>
         <v>0.39768557719446795</v>
       </c>
       <c r="AM22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.51475000000000004</v>
       </c>
       <c r="AN22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.52032710280373828</v>
       </c>
       <c r="AO22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.54915254237288136</v>
       </c>
       <c r="AP22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.5552232428968169</v>
       </c>
       <c r="AQ22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.61206896551724133</v>
       </c>
       <c r="AR22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.61989375343469499</v>
       </c>
       <c r="AS22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.59934115709285563</v>
       </c>
       <c r="AT22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.61206896551724133</v>
       </c>
       <c r="AU22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.61989375343469499</v>
       </c>
       <c r="AV22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.65046109043844036</v>
       </c>
       <c r="AW22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.64929033216913135</v>
       </c>
       <c r="AX22" s="8">
-        <f t="shared" si="83"/>
+        <f t="shared" si="132"/>
         <v>0.56928894490991322</v>
       </c>
-      <c r="AY22" s="8"/>
+      <c r="AY22" s="8">
+        <f t="shared" ref="AY22" si="133">AY7/AY5</f>
+        <v>0.72717573290436954</v>
+      </c>
       <c r="AZ22" s="8"/>
       <c r="BA22" s="8"/>
       <c r="BB22" s="8"/>
@@ -4280,106 +4270,109 @@
         <v>-1.6582569701696248E-2</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" ref="G23:AE23" si="84">G22/F22-1</f>
+        <f t="shared" ref="G23:AF23" si="134">G22/F22-1</f>
         <v>1.946287840115235E-2</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>3.9426942353338212E-2</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>4.2269591071862456E-2</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-1.9283366499627475E-2</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-4.5076502493046178E-2</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-9.3568518852968907E-2</v>
       </c>
       <c r="M23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>6.6481560267807049E-2</v>
       </c>
       <c r="N23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>2.3526919707609784E-2</v>
       </c>
       <c r="O23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>6.3900370626025271E-2</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>2.0848251355648939E-2</v>
       </c>
       <c r="Q23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>2.6135155167414936E-3</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-9.5575016547350233E-2</v>
       </c>
       <c r="S23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-2.491801930529669E-3</v>
       </c>
       <c r="T23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>0.12687208254822258</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-3.0867476031291585E-2</v>
       </c>
       <c r="V23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>1.0468917400058952E-2</v>
       </c>
       <c r="W23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>6.5055966027085521E-3</v>
       </c>
       <c r="X23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>3.3978784357548975E-3</v>
       </c>
       <c r="Y23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>1.6682673745171961E-3</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>-0.33644871723320857</v>
       </c>
       <c r="AA23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>0.23192632946118774</v>
       </c>
       <c r="AB23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>0.182557796033058</v>
       </c>
       <c r="AC23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>2.0245703040773222E-2</v>
       </c>
       <c r="AD23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>8.3945890490644937E-2</v>
       </c>
       <c r="AE23" s="8">
-        <f t="shared" si="84"/>
+        <f t="shared" si="134"/>
         <v>5.5656342110629087E-2</v>
       </c>
-      <c r="AF23" s="8"/>
+      <c r="AF23" s="8">
+        <f t="shared" si="134"/>
+        <v>2.725610962515379E-2</v>
+      </c>
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
       <c r="AI23" s="8"/>
@@ -4387,54 +4380,57 @@
       <c r="AK23" s="8"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
-        <f t="shared" ref="AM23" si="85">AM22/AL22-1</f>
+        <f t="shared" ref="AM23" si="135">AM22/AL22-1</f>
         <v>0.29436426543647998</v>
       </c>
       <c r="AN23" s="8">
-        <f t="shared" ref="AN23" si="86">AN22/AM22-1</f>
+        <f t="shared" ref="AN23" si="136">AN22/AM22-1</f>
         <v>1.0834585339948077E-2</v>
       </c>
       <c r="AO23" s="8">
-        <f t="shared" ref="AO23" si="87">AO22/AN22-1</f>
+        <f t="shared" ref="AO23" si="137">AO22/AN22-1</f>
         <v>5.5398689427899495E-2</v>
       </c>
       <c r="AP23" s="8">
-        <f t="shared" ref="AP23" si="88">AP22/AO22-1</f>
+        <f t="shared" ref="AP23" si="138">AP22/AO22-1</f>
         <v>1.1054670707166592E-2</v>
       </c>
       <c r="AQ23" s="8">
-        <f t="shared" ref="AQ23" si="89">AQ22/AP22-1</f>
+        <f t="shared" ref="AQ23" si="139">AQ22/AP22-1</f>
         <v>0.10238354274190331</v>
       </c>
       <c r="AR23" s="8">
-        <f t="shared" ref="AR23" si="90">AR22/AQ22-1</f>
+        <f t="shared" ref="AR23" si="140">AR22/AQ22-1</f>
         <v>1.2784160541191802E-2</v>
       </c>
       <c r="AS23" s="8">
-        <f t="shared" ref="AS23" si="91">AS22/AR22-1</f>
+        <f t="shared" ref="AS23" si="141">AS22/AR22-1</f>
         <v>-3.3155030564450683E-2</v>
       </c>
       <c r="AT23" s="8">
-        <f t="shared" ref="AT23" si="92">AT22/AS22-1</f>
+        <f t="shared" ref="AT23" si="142">AT22/AS22-1</f>
         <v>2.1236333052985668E-2</v>
       </c>
       <c r="AU23" s="8">
-        <f t="shared" ref="AU23" si="93">AU22/AT22-1</f>
+        <f t="shared" ref="AU23" si="143">AU22/AT22-1</f>
         <v>1.2784160541191802E-2</v>
       </c>
       <c r="AV23" s="8">
-        <f t="shared" ref="AV23" si="94">AV22/AU22-1</f>
+        <f t="shared" ref="AV23" si="144">AV22/AU22-1</f>
         <v>4.9310606590852846E-2</v>
       </c>
       <c r="AW23" s="8">
-        <f t="shared" ref="AW23" si="95">AW22/AV22-1</f>
+        <f t="shared" ref="AW23" si="145">AW22/AV22-1</f>
         <v>-1.7998897805245884E-3</v>
       </c>
       <c r="AX23" s="8">
-        <f t="shared" ref="AX23" si="96">AX22/AW22-1</f>
+        <f t="shared" ref="AX23:AY23" si="146">AX22/AW22-1</f>
         <v>-0.12321358149897543</v>
       </c>
-      <c r="AY23" s="8"/>
+      <c r="AY23" s="8">
+        <f t="shared" si="146"/>
+        <v>0.27734033728591201</v>
+      </c>
       <c r="AZ23" s="8"/>
       <c r="BA23" s="8"/>
       <c r="BB23" s="8"/>
@@ -4580,106 +4576,109 @@
         <v>0.16455696202531644</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" ref="G26:AE26" si="97">G15/F15-1</f>
+        <f t="shared" ref="G26:AF26" si="147">G15/F15-1</f>
         <v>0.44565217391304346</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.33834586466165417</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.11235955056179758</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.11111111111111105</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.14772727272727271</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.48019801980198007</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.39047619047619064</v>
       </c>
       <c r="N26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.421875</v>
       </c>
       <c r="O26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.6153846153846152</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>2.0408163265305923E-2</v>
       </c>
       <c r="Q26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-1.9999999999999685E-2</v>
       </c>
       <c r="R26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.32653061224489799</v>
       </c>
       <c r="S26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>1.1414141414141414</v>
       </c>
       <c r="T26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>9.4339622641509413E-2</v>
       </c>
       <c r="U26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.30603448275862055</v>
       </c>
       <c r="V26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.68976897689768979</v>
       </c>
       <c r="W26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>3.1914893617021267E-2</v>
       </c>
       <c r="X26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.12371134020618557</v>
       </c>
       <c r="Y26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.41284403669724778</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>-0.59375</v>
       </c>
       <c r="AA26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>3.8461538461538547E-2</v>
       </c>
       <c r="AB26" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="AC26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.43859649122806998</v>
       </c>
       <c r="AD26" s="7">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>2.0487804878048781</v>
       </c>
       <c r="AE26" s="8">
-        <f t="shared" si="97"/>
+        <f t="shared" si="147"/>
         <v>0.5</v>
       </c>
-      <c r="AF26" s="8"/>
+      <c r="AF26" s="8">
+        <f t="shared" si="147"/>
+        <v>0.31466666666666665</v>
+      </c>
       <c r="AG26" s="8"/>
       <c r="AH26" s="8"/>
       <c r="AI26" s="8"/>

</xml_diff>